<commit_message>
fix(Examples): Update `coral-reef-light` configuration and storage files
</commit_message>
<xml_diff>
--- a/examples/campaigns/coral-reef-light/coral-reef-light.xlsx
+++ b/examples/campaigns/coral-reef-light/coral-reef-light.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Help" sheetId="1" state="visible" r:id="rId2"/>
@@ -573,7 +573,7 @@
     <t xml:space="preserve">value</t>
   </si>
   <si>
-    <t xml:space="preserve">coral-reef.h5</t>
+    <t xml:space="preserve">coral-reef-light.h5</t>
   </si>
   <si>
     <t xml:space="preserve">audio</t>
@@ -1275,192 +1275,196 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1537,14 +1541,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFDDDDDD"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:B60"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="5" topLeftCell="B6" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -1938,7 +1942,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1947,7 +1951,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFB4C7DC"/>
     <pageSetUpPr fitToPage="false"/>
@@ -1975,16 +1979,16 @@
       <c r="B1" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="F1" s="0"/>
+      <c r="F1" s="40"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="36" t="s">
@@ -1993,9 +1997,9 @@
       <c r="B2" s="38" t="n">
         <v>2</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="36" t="s">
@@ -2007,18 +2011,18 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1" type="none">
       <formula1>ListAutoclusters!$A$2:$A$1048576</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1003" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1003" type="list">
       <formula1>ListReducers!$A$2:$A$1048576</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2028,7 +2032,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFB4C7DC"/>
     <pageSetUpPr fitToPage="false"/>
@@ -2069,7 +2073,7 @@
       <c r="E1" s="39" t="s">
         <v>210</v>
       </c>
-      <c r="F1" s="0"/>
+      <c r="F1" s="40"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="36" t="s">
@@ -2107,18 +2111,18 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1" type="none">
       <formula1>ListAutoclusters!$A$2:$A$1048576</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1002" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1002" type="list">
       <formula1>ListAutoclusters!$A$2:$A$1048576</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2127,7 +2131,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFDDDDDD"/>
     <pageSetUpPr fitToPage="false"/>
@@ -2145,15 +2149,15 @@
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="15" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="42" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="43" width="42.79"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="44" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="45" t="s">
         <v>214</v>
       </c>
     </row>
@@ -2161,7 +2165,7 @@
       <c r="A2" s="15" t="s">
         <v>198</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="46" t="s">
         <v>215</v>
       </c>
     </row>
@@ -2169,7 +2173,7 @@
       <c r="A3" s="15" t="s">
         <v>216</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="46" t="s">
         <v>217</v>
       </c>
     </row>
@@ -2177,7 +2181,7 @@
       <c r="A4" s="15" t="s">
         <v>218</v>
       </c>
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="46" t="s">
         <v>219</v>
       </c>
     </row>
@@ -2185,7 +2189,7 @@
       <c r="A5" s="15" t="s">
         <v>220</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="46" t="s">
         <v>221</v>
       </c>
     </row>
@@ -2193,7 +2197,7 @@
       <c r="A6" s="15" t="s">
         <v>222</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="46" t="s">
         <v>223</v>
       </c>
     </row>
@@ -2201,7 +2205,7 @@
       <c r="A7" s="15" t="s">
         <v>224</v>
       </c>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="47" t="s">
         <v>225</v>
       </c>
     </row>
@@ -2209,7 +2213,7 @@
       <c r="A8" s="15" t="s">
         <v>202</v>
       </c>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="47" t="s">
         <v>226</v>
       </c>
     </row>
@@ -2217,7 +2221,7 @@
       <c r="A9" s="15" t="s">
         <v>227</v>
       </c>
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="47" t="s">
         <v>228</v>
       </c>
     </row>
@@ -2225,14 +2229,14 @@
       <c r="A10" s="15" t="s">
         <v>200</v>
       </c>
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="47" t="s">
         <v>229</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2241,7 +2245,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFDDDDDD"/>
     <pageSetUpPr fitToPage="false"/>
@@ -2259,15 +2263,15 @@
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="15" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="42" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="43" width="42.79"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="44" t="s">
         <v>230</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="45" t="s">
         <v>214</v>
       </c>
     </row>
@@ -2275,7 +2279,7 @@
       <c r="A2" s="15" t="s">
         <v>231</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="46" t="s">
         <v>232</v>
       </c>
     </row>
@@ -2283,7 +2287,7 @@
       <c r="A3" s="15" t="s">
         <v>233</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="46" t="s">
         <v>234</v>
       </c>
     </row>
@@ -2291,7 +2295,7 @@
       <c r="A4" s="15" t="s">
         <v>235</v>
       </c>
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="46" t="s">
         <v>236</v>
       </c>
     </row>
@@ -2299,7 +2303,7 @@
       <c r="A5" s="15" t="s">
         <v>237</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="46" t="s">
         <v>238</v>
       </c>
     </row>
@@ -2307,7 +2311,7 @@
       <c r="A6" s="15" t="s">
         <v>239</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="46" t="s">
         <v>240</v>
       </c>
     </row>
@@ -2315,7 +2319,7 @@
       <c r="A7" s="15" t="s">
         <v>204</v>
       </c>
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="46" t="s">
         <v>241</v>
       </c>
     </row>
@@ -2323,7 +2327,7 @@
       <c r="A8" s="15" t="s">
         <v>203</v>
       </c>
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="46" t="s">
         <v>242</v>
       </c>
     </row>
@@ -2331,17 +2335,17 @@
       <c r="A9" s="15" t="s">
         <v>205</v>
       </c>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="46" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="46"/>
+      <c r="B10" s="47"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2350,7 +2354,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFDDDDDD"/>
     <pageSetUpPr fitToPage="false"/>
@@ -2372,7 +2376,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="44" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2389,7 +2393,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2398,7 +2402,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFDDDDDD"/>
     <pageSetUpPr fitToPage="false"/>
@@ -2416,7 +2420,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="44" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2438,7 +2442,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2447,7 +2451,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFDDDDDD"/>
     <pageSetUpPr fitToPage="false"/>
@@ -2469,7 +2473,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="44" t="s">
         <v>72</v>
       </c>
     </row>
@@ -2496,7 +2500,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2505,14 +2509,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFA6"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -2522,8 +2526,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="29.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="48.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="29.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="48.94"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="3" style="1" width="11.52"/>
   </cols>
   <sheetData>
@@ -2611,7 +2615,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2620,7 +2624,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFA6"/>
     <pageSetUpPr fitToPage="false"/>
@@ -2638,7 +2642,7 @@
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="24" width="56.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="63.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="63.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="26" width="22.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="4" style="27" width="20.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="11" style="28" width="15.84"/>
@@ -5894,7 +5898,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -5903,7 +5907,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFA6"/>
     <pageSetUpPr fitToPage="false"/>
@@ -5962,7 +5966,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -5971,7 +5975,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFA6"/>
     <pageSetUpPr fitToPage="false"/>
@@ -6021,7 +6025,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -6030,7 +6034,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFA6"/>
     <pageSetUpPr fitToPage="false"/>
@@ -6110,7 +6114,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -6119,7 +6123,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFFFFA6"/>
     <pageSetUpPr fitToPage="false"/>
@@ -6227,14 +6231,14 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F2:F1004" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F2:F1004" type="list">
       <formula1>ListTrajectories!$A$2:$A$1048576</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -6243,7 +6247,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFB4C7DC"/>
     <pageSetUpPr fitToPage="false"/>
@@ -6256,7 +6260,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="36" width="10.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="36" width="10.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="37" width="14.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="38" width="17.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="38" width="15.45"/>
@@ -6276,7 +6280,7 @@
       <c r="D1" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="E1" s="0"/>
+      <c r="E1" s="40"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="36" t="s">
@@ -6322,14 +6326,14 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1001" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1001" type="list">
       <formula1>ListExtractors!$A$2:$A$1048576</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -6339,7 +6343,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFB4C7DC"/>
     <pageSetUpPr fitToPage="false"/>
@@ -6378,18 +6382,18 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A1" type="none">
       <formula1>Help!$A$2:$A$1048576</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1004" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1004" type="list">
       <formula1>ListDigesters!$A$2:$A$1048576</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
fix(Examples/CoralReefLight): Translate files labels to english
</commit_message>
<xml_diff>
--- a/examples/campaigns/coral-reef-light/coral-reef-light.xlsx
+++ b/examples/campaigns/coral-reef-light/coral-reef-light.xlsx
@@ -615,7 +615,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="194">
   <si>
     <t xml:space="preserve">SoundScapeExplorer
 Version 12</t>
@@ -811,10 +811,10 @@
     <t xml:space="preserve">date</t>
   </si>
   <si>
-    <t xml:space="preserve">label_LIEU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">label_ANNEE</t>
+    <t xml:space="preserve">label_LOCATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">label_YEAR</t>
   </si>
   <si>
     <t xml:space="preserve">label_REPLICA</t>
@@ -823,31 +823,31 @@
     <t xml:space="preserve">label_SNAP</t>
   </si>
   <si>
-    <t xml:space="preserve">label_PROFONDEUR</t>
+    <t xml:space="preserve">label_DEPTH</t>
   </si>
   <si>
     <t xml:space="preserve">label_GEOMORPH</t>
   </si>
   <si>
-    <t xml:space="preserve">label_SUBSTRAT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">label_PERIODE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">label_BATEAU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">label_PLUIE</t>
+    <t xml:space="preserve">label_SUBSTRATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">label_PERIOD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">label_BOAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">label_RAIN</t>
   </si>
   <si>
     <t xml:space="preserve">label_SONAR</t>
   </si>
   <si>
-    <t xml:space="preserve">label_ABONDANCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">label_RICHESSE</t>
+    <t xml:space="preserve">label_ABUNDANCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">label_RICHNESS</t>
   </si>
   <si>
     <t xml:space="preserve">label_ABVOCAL</t>
@@ -856,34 +856,31 @@
     <t xml:space="preserve">label_RVOCAL</t>
   </si>
   <si>
-    <t xml:space="preserve">label_LIEU+ANNEE+REPLICA</t>
+    <t xml:space="preserve">label_LOCATION+YEAR+REPLICA</t>
   </si>
   <si>
     <t xml:space="preserve">/2022_passe_1/data_filtree/20221116T120500_2614231302179085_2.0.wav</t>
   </si>
   <si>
-    <t xml:space="preserve">passe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chenal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dalle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jour</t>
-  </si>
-  <si>
-    <t xml:space="preserve">non</t>
-  </si>
-  <si>
-    <t xml:space="preserve">passe/2022/1</t>
+    <t xml:space="preserve">boat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">channel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no</t>
   </si>
   <si>
     <t xml:space="preserve">/2022_passe_1/data_filtree/20221116T121500_2614231302179085_2.0.wav</t>
   </si>
   <si>
-    <t xml:space="preserve">oui</t>
+    <t xml:space="preserve">yes</t>
   </si>
   <si>
     <t xml:space="preserve">/2022_passe_1/data_filtree/20221116T122500_2614231302179085_2.0.wav</t>
@@ -892,9 +889,6 @@
     <t xml:space="preserve">/2022_passe_2/data_filtree/20221122T120000_2614231302179085_2.0.wav</t>
   </si>
   <si>
-    <t xml:space="preserve">passe/2022/2</t>
-  </si>
-  <si>
     <t xml:space="preserve">/2022_passe_2/data_filtree/20221122T121000_2614231302179085_2.0.wav</t>
   </si>
   <si>
@@ -904,9 +898,6 @@
     <t xml:space="preserve">/2022_passe_3/data_filtree/20221212T120500_2614231302179085_2.0.wav</t>
   </si>
   <si>
-    <t xml:space="preserve">passe/2022/3</t>
-  </si>
-  <si>
     <t xml:space="preserve">/2022_passe_3/data_filtree/20221212T121500_2614231302179085_2.0.wav</t>
   </si>
   <si>
@@ -916,16 +907,13 @@
     <t xml:space="preserve">/2022_naturel_1/data_filtree/20221116T120500_4407951432584596_2.0.wav</t>
   </si>
   <si>
-    <t xml:space="preserve">naturel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">barriere</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">naturel/2022/1</t>
+    <t xml:space="preserve">undegraded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">barrier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sand</t>
   </si>
   <si>
     <t xml:space="preserve">/2022_naturel_1/data_filtree/20221116T121500_4407951432584596_2.0.wav</t>
@@ -937,9 +925,6 @@
     <t xml:space="preserve">/2022_naturel_2/data_filtree/20221122T120500_4407951432584596_2.0.wav</t>
   </si>
   <si>
-    <t xml:space="preserve">naturel/2022/2</t>
-  </si>
-  <si>
     <t xml:space="preserve">/2022_naturel_2/data_filtree/20221122T121500_4407951432584596_2.0.wav</t>
   </si>
   <si>
@@ -949,9 +934,6 @@
     <t xml:space="preserve">/2022_naturel_3/data_filtree/20221212T120000_4407951432584596_2.0.wav</t>
   </si>
   <si>
-    <t xml:space="preserve">naturel/2022/3</t>
-  </si>
-  <si>
     <t xml:space="preserve">/2022_naturel_3/data_filtree/20221212T121000_4407951432584596_2.0.wav</t>
   </si>
   <si>
@@ -961,10 +943,7 @@
     <t xml:space="preserve">/2022_touriste_1/data_filtree/20221116T120000_2614231121130510_2.0.wav</t>
   </si>
   <si>
-    <t xml:space="preserve">touriste</t>
-  </si>
-  <si>
-    <t xml:space="preserve">touriste/2022/1</t>
+    <t xml:space="preserve">tourist</t>
   </si>
   <si>
     <t xml:space="preserve">/2022_touriste_1/data_filtree/20221116T121000_2614231121130510_2.0.wav</t>
@@ -976,9 +955,6 @@
     <t xml:space="preserve">/2022_touriste_2/data_filtree/20221122T120500_2614231121130510_2.0.wav</t>
   </si>
   <si>
-    <t xml:space="preserve">touriste/2022/2</t>
-  </si>
-  <si>
     <t xml:space="preserve">/2022_touriste_2/data_filtree/20221122T121500_2614231121130510_2.0.wav</t>
   </si>
   <si>
@@ -988,9 +964,6 @@
     <t xml:space="preserve">/2022_touriste_3/data_filtree/20221212T120500_2614231121130510_2.0.wav</t>
   </si>
   <si>
-    <t xml:space="preserve">touriste/2022/3</t>
-  </si>
-  <si>
     <t xml:space="preserve">/2022_touriste_3/data_filtree/20221212T121500_2614231121130510_2.0.wav</t>
   </si>
   <si>
@@ -1000,9 +973,6 @@
     <t xml:space="preserve">/2021_naturel_1/data_filtree/20210216T120200_2614231302179085_2.0.wav</t>
   </si>
   <si>
-    <t xml:space="preserve">naturel/2021/1</t>
-  </si>
-  <si>
     <t xml:space="preserve">/2021_naturel_1/data_filtree/20210216T121300_2614231302179085_2.0.wav</t>
   </si>
   <si>
@@ -1012,9 +982,6 @@
     <t xml:space="preserve">/2021_naturel_2/data_filtree/20210318T120500_2614231121130510_2.0.wav</t>
   </si>
   <si>
-    <t xml:space="preserve">naturel/2021/2</t>
-  </si>
-  <si>
     <t xml:space="preserve">/2021_naturel_2/data_filtree/20210318T121600_2614231121130510_2.0.wav</t>
   </si>
   <si>
@@ -1024,9 +991,6 @@
     <t xml:space="preserve">/2021_naturel_3/data_filtree/20210414T120500_2614231112834446_2.0.wav</t>
   </si>
   <si>
-    <t xml:space="preserve">naturel/2021/3</t>
-  </si>
-  <si>
     <t xml:space="preserve">/2021_naturel_3/data_filtree/20210414T121600_2614231112834446_2.0.wav</t>
   </si>
   <si>
@@ -1036,9 +1000,6 @@
     <t xml:space="preserve">/2021_passe_1/data_filtree/20210218T120600_2614231302179085_2.0.wav</t>
   </si>
   <si>
-    <t xml:space="preserve">passe/2021/1</t>
-  </si>
-  <si>
     <t xml:space="preserve">/2021_passe_1/data_filtree/20210218T121700_2614231302179085_2.0.wav</t>
   </si>
   <si>
@@ -1048,9 +1009,6 @@
     <t xml:space="preserve">/2021_passe_2/data_filtree/20210316T120400_2614231302179085_2.0.wav</t>
   </si>
   <si>
-    <t xml:space="preserve">passe/2021/2</t>
-  </si>
-  <si>
     <t xml:space="preserve">/2021_passe_2/data_filtree/20210316T121500_2614231302179085_2.0.wav</t>
   </si>
   <si>
@@ -1060,9 +1018,6 @@
     <t xml:space="preserve">/2021_passe_3/data_filtree/20210419T120400_2614231112834446_2.0.wav</t>
   </si>
   <si>
-    <t xml:space="preserve">passe/2021/3</t>
-  </si>
-  <si>
     <t xml:space="preserve">/2021_passe_3/data_filtree/20210419T121500_2614231112834446_2.0.wav</t>
   </si>
   <si>
@@ -1072,9 +1027,6 @@
     <t xml:space="preserve">/2021_touriste_1/data_filtree/20210216T120800_2614231121130510_2.0.wav</t>
   </si>
   <si>
-    <t xml:space="preserve">touriste/2021/1</t>
-  </si>
-  <si>
     <t xml:space="preserve">/2021_touriste_1/data_filtree/20210216T121900_2614231121130510_2.0.wav</t>
   </si>
   <si>
@@ -1084,9 +1036,6 @@
     <t xml:space="preserve">/2021_touriste_2/data_filtree/20210318T120000_2614231302179085_2.0.wav</t>
   </si>
   <si>
-    <t xml:space="preserve">touriste/2021/2</t>
-  </si>
-  <si>
     <t xml:space="preserve">/2021_touriste_2/data_filtree/20210318T121100_2614231302179085_2.0.wav</t>
   </si>
   <si>
@@ -1096,9 +1045,6 @@
     <t xml:space="preserve">/2021_touriste_3/data_filtree/20210413T121000_2614231302179085_2.0.wav</t>
   </si>
   <si>
-    <t xml:space="preserve">touriste/2021/3</t>
-  </si>
-  <si>
     <t xml:space="preserve">/2021_touriste_3/data_filtree/20210413T122100_2614231302179085_2.0.wav</t>
   </si>
   <si>
@@ -1162,7 +1108,7 @@
     <t xml:space="preserve">day1</t>
   </si>
   <si>
-    <t xml:space="preserve">LIEU</t>
+    <t xml:space="preserve">LOCATION</t>
   </si>
   <si>
     <t xml:space="preserve">hour</t>
@@ -1186,9 +1132,6 @@
     <t xml:space="preserve">vgg</t>
   </si>
   <si>
-    <t xml:space="preserve">no</t>
-  </si>
-  <si>
     <t xml:space="preserve">digester</t>
   </si>
   <si>
@@ -1340,9 +1283,6 @@
   </si>
   <si>
     <t xml:space="preserve">pca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">day</t>
   </si>
   <si>
     <t xml:space="preserve">month</t>
@@ -1957,24 +1897,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="40" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
       <c r="B1" s="40" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="C1" s="42" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="D1" s="42" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="E1" s="42" t="s">
-        <v>168</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="36" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="B2" s="38" t="n">
         <v>2</v>
@@ -1985,7 +1925,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="36" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="B3" s="37" t="n">
         <v>3</v>
@@ -2039,24 +1979,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="40" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="B1" s="40" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
       <c r="C1" s="40" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="D1" s="40" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="E1" s="40" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="36" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="B2" s="38" t="n">
         <v>15</v>
@@ -2073,7 +2013,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="36" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="B3" s="37" t="n">
         <v>15</v>
@@ -2094,12 +2034,12 @@
       <formula1>ListAutoclusters!$A$2:$A$1048576</formula1>
       <formula2>0</formula2>
     </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A3" type="list">
+      <formula1>ListReducers!$A$2:$A$1048576</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A4:A1002" type="list">
       <formula1>ListAutoclusters!$A$2:$A$1048576</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A3" type="list">
-      <formula1>ListReducers!$A$2:$A$1048576</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -2139,82 +2079,82 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="46" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="B1" s="47" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="44" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
       <c r="B2" s="48" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="44" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="44" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="B4" s="48" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="44" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="B5" s="48" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="44" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
       <c r="B6" s="48" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="44" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="B7" s="49" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="44" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="B8" s="49" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="44" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="B9" s="49" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="44" t="s">
-        <v>194</v>
+        <v>175</v>
       </c>
       <c r="B10" s="49" t="s">
-        <v>195</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -2253,74 +2193,74 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="46" t="s">
-        <v>196</v>
+        <v>177</v>
       </c>
       <c r="B1" s="47" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="44" t="s">
-        <v>197</v>
+        <v>178</v>
       </c>
       <c r="B2" s="48" t="s">
-        <v>198</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="44" t="s">
-        <v>199</v>
+        <v>180</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="44" t="s">
-        <v>201</v>
+        <v>182</v>
       </c>
       <c r="B4" s="48" t="s">
-        <v>202</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="44" t="s">
-        <v>203</v>
+        <v>184</v>
       </c>
       <c r="B5" s="48" t="s">
-        <v>204</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="44" t="s">
-        <v>205</v>
+        <v>186</v>
       </c>
       <c r="B6" s="48" t="s">
-        <v>206</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="44" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
       <c r="B7" s="48" t="s">
-        <v>208</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="44" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="B8" s="48" t="s">
-        <v>209</v>
+        <v>190</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="44" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
       <c r="B9" s="48" t="s">
-        <v>210</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2361,17 +2301,17 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="46" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="44" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="44" t="s">
-        <v>211</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -2409,17 +2349,17 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="46" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="44" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="44" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -2453,22 +2393,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="46" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="44" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="44" t="s">
-        <v>212</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="44" t="s">
-        <v>213</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -3675,7 +3615,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="24" width="42.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="25" width="22.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="26" width="20.56"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="28" min="5" style="27" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="5" style="27" width="18.21"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="28" min="20" style="27" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1003" min="29" style="1" width="11.52"/>
   </cols>
   <sheetData>
@@ -3793,16 +3734,17 @@
       <c r="R2" s="27" t="n">
         <v>58</v>
       </c>
-      <c r="S2" s="27" t="s">
-        <v>57</v>
+      <c r="S2" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D2,"/",E2,"/",F2)</f>
+        <v>boat/2022/1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" s="31" t="n">
         <v>44881.5104166667</v>
@@ -3832,7 +3774,7 @@
         <v>55</v>
       </c>
       <c r="L3" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M3" s="27" t="s">
         <v>56</v>
@@ -3852,16 +3794,17 @@
       <c r="R3" s="27" t="n">
         <v>58</v>
       </c>
-      <c r="S3" s="27" t="s">
-        <v>57</v>
+      <c r="S3" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D3,"/",E3,"/",F3)</f>
+        <v>boat/2022/1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C4" s="31" t="n">
         <v>44881.5173611111</v>
@@ -3891,7 +3834,7 @@
         <v>55</v>
       </c>
       <c r="L4" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M4" s="27" t="s">
         <v>56</v>
@@ -3911,16 +3854,17 @@
       <c r="R4" s="27" t="n">
         <v>58</v>
       </c>
-      <c r="S4" s="27" t="s">
-        <v>57</v>
+      <c r="S4" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D4,"/",E4,"/",F4)</f>
+        <v>boat/2022/1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C5" s="32" t="n">
         <v>44887.5</v>
@@ -3950,7 +3894,7 @@
         <v>55</v>
       </c>
       <c r="L5" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M5" s="27" t="s">
         <v>56</v>
@@ -3970,16 +3914,17 @@
       <c r="R5" s="27" t="n">
         <v>58</v>
       </c>
-      <c r="S5" s="27" t="s">
-        <v>62</v>
+      <c r="S5" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D5,"/",E5,"/",F5)</f>
+        <v>boat/2022/2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="29" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C6" s="32" t="n">
         <v>44887.5069444444</v>
@@ -4009,7 +3954,7 @@
         <v>55</v>
       </c>
       <c r="L6" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M6" s="27" t="s">
         <v>56</v>
@@ -4029,16 +3974,17 @@
       <c r="R6" s="27" t="n">
         <v>58</v>
       </c>
-      <c r="S6" s="27" t="s">
-        <v>62</v>
+      <c r="S6" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D6,"/",E6,"/",F6)</f>
+        <v>boat/2022/2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="23" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C7" s="32" t="n">
         <v>44887.5138888889</v>
@@ -4068,7 +4014,7 @@
         <v>55</v>
       </c>
       <c r="L7" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M7" s="27" t="s">
         <v>56</v>
@@ -4088,16 +4034,17 @@
       <c r="R7" s="27" t="n">
         <v>58</v>
       </c>
-      <c r="S7" s="27" t="s">
-        <v>62</v>
+      <c r="S7" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D7,"/",E7,"/",F7)</f>
+        <v>boat/2022/2</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C8" s="32" t="n">
         <v>44907.5034722222</v>
@@ -4127,7 +4074,7 @@
         <v>55</v>
       </c>
       <c r="L8" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M8" s="27" t="s">
         <v>56</v>
@@ -4147,16 +4094,17 @@
       <c r="R8" s="27" t="n">
         <v>58</v>
       </c>
-      <c r="S8" s="27" t="s">
-        <v>66</v>
+      <c r="S8" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D8,"/",E8,"/",F8)</f>
+        <v>boat/2022/3</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="23" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C9" s="32" t="n">
         <v>44907.5104166667</v>
@@ -4186,7 +4134,7 @@
         <v>55</v>
       </c>
       <c r="L9" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M9" s="27" t="s">
         <v>56</v>
@@ -4206,16 +4154,17 @@
       <c r="R9" s="27" t="n">
         <v>58</v>
       </c>
-      <c r="S9" s="27" t="s">
-        <v>66</v>
+      <c r="S9" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D9,"/",E9,"/",F9)</f>
+        <v>boat/2022/3</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="23" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C10" s="32" t="n">
         <v>44907.5173611111</v>
@@ -4245,7 +4194,7 @@
         <v>55</v>
       </c>
       <c r="L10" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M10" s="27" t="s">
         <v>56</v>
@@ -4265,22 +4214,23 @@
       <c r="R10" s="27" t="n">
         <v>58</v>
       </c>
-      <c r="S10" s="27" t="s">
-        <v>66</v>
+      <c r="S10" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D10,"/",E10,"/",F10)</f>
+        <v>boat/2022/3</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="23" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C11" s="32" t="n">
         <v>44881.5034722222</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E11" s="26" t="n">
         <v>2022</v>
@@ -4295,10 +4245,10 @@
         <v>2</v>
       </c>
       <c r="I11" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J11" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K11" s="27" t="s">
         <v>55</v>
@@ -4324,22 +4274,23 @@
       <c r="R11" s="27" t="n">
         <v>44</v>
       </c>
-      <c r="S11" s="27" t="s">
-        <v>73</v>
+      <c r="S11" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D11,"/",E11,"/",F11)</f>
+        <v>undegraded/2022/1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="23" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C12" s="32" t="n">
         <v>44881.5104166667</v>
       </c>
       <c r="D12" s="26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E12" s="26" t="n">
         <v>2022</v>
@@ -4354,10 +4305,10 @@
         <v>2</v>
       </c>
       <c r="I12" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J12" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K12" s="27" t="s">
         <v>55</v>
@@ -4383,22 +4334,23 @@
       <c r="R12" s="27" t="n">
         <v>44</v>
       </c>
-      <c r="S12" s="27" t="s">
-        <v>73</v>
+      <c r="S12" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D12,"/",E12,"/",F12)</f>
+        <v>undegraded/2022/1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C13" s="32" t="n">
         <v>44881.5173611111</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E13" s="26" t="n">
         <v>2022</v>
@@ -4413,10 +4365,10 @@
         <v>2</v>
       </c>
       <c r="I13" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J13" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K13" s="27" t="s">
         <v>55</v>
@@ -4442,22 +4394,23 @@
       <c r="R13" s="27" t="n">
         <v>44</v>
       </c>
-      <c r="S13" s="27" t="s">
-        <v>73</v>
+      <c r="S13" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D13,"/",E13,"/",F13)</f>
+        <v>undegraded/2022/1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C14" s="32" t="n">
         <v>44887.5034722222</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E14" s="26" t="n">
         <v>2022</v>
@@ -4472,10 +4425,10 @@
         <v>2</v>
       </c>
       <c r="I14" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J14" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K14" s="27" t="s">
         <v>55</v>
@@ -4501,22 +4454,23 @@
       <c r="R14" s="27" t="n">
         <v>44</v>
       </c>
-      <c r="S14" s="27" t="s">
-        <v>77</v>
+      <c r="S14" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D14,"/",E14,"/",F14)</f>
+        <v>undegraded/2022/2</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="23" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C15" s="32" t="n">
         <v>44887.5104166667</v>
       </c>
       <c r="D15" s="26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E15" s="26" t="n">
         <v>2022</v>
@@ -4531,10 +4485,10 @@
         <v>2</v>
       </c>
       <c r="I15" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J15" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K15" s="27" t="s">
         <v>55</v>
@@ -4560,22 +4514,23 @@
       <c r="R15" s="27" t="n">
         <v>44</v>
       </c>
-      <c r="S15" s="27" t="s">
-        <v>77</v>
+      <c r="S15" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D15,"/",E15,"/",F15)</f>
+        <v>undegraded/2022/2</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="23" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C16" s="32" t="n">
         <v>44887.5173611111</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E16" s="26" t="n">
         <v>2022</v>
@@ -4590,10 +4545,10 @@
         <v>2</v>
       </c>
       <c r="I16" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J16" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K16" s="27" t="s">
         <v>55</v>
@@ -4619,22 +4574,23 @@
       <c r="R16" s="27" t="n">
         <v>44</v>
       </c>
-      <c r="S16" s="27" t="s">
-        <v>77</v>
+      <c r="S16" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D16,"/",E16,"/",F16)</f>
+        <v>undegraded/2022/2</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="23" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C17" s="32" t="n">
         <v>44907.5</v>
       </c>
       <c r="D17" s="26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E17" s="26" t="n">
         <v>2022</v>
@@ -4649,10 +4605,10 @@
         <v>2</v>
       </c>
       <c r="I17" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J17" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K17" s="27" t="s">
         <v>55</v>
@@ -4678,22 +4634,23 @@
       <c r="R17" s="27" t="n">
         <v>44</v>
       </c>
-      <c r="S17" s="27" t="s">
-        <v>81</v>
+      <c r="S17" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D17,"/",E17,"/",F17)</f>
+        <v>undegraded/2022/3</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="23" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C18" s="32" t="n">
         <v>44907.5069444444</v>
       </c>
       <c r="D18" s="26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E18" s="26" t="n">
         <v>2022</v>
@@ -4708,10 +4665,10 @@
         <v>2</v>
       </c>
       <c r="I18" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J18" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K18" s="27" t="s">
         <v>55</v>
@@ -4737,22 +4694,23 @@
       <c r="R18" s="27" t="n">
         <v>44</v>
       </c>
-      <c r="S18" s="27" t="s">
-        <v>81</v>
+      <c r="S18" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D18,"/",E18,"/",F18)</f>
+        <v>undegraded/2022/3</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="23" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C19" s="32" t="n">
         <v>44907.5138888889</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E19" s="26" t="n">
         <v>2022</v>
@@ -4767,10 +4725,10 @@
         <v>2</v>
       </c>
       <c r="I19" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J19" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K19" s="27" t="s">
         <v>55</v>
@@ -4796,22 +4754,23 @@
       <c r="R19" s="27" t="n">
         <v>44</v>
       </c>
-      <c r="S19" s="27" t="s">
-        <v>81</v>
+      <c r="S19" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D19,"/",E19,"/",F19)</f>
+        <v>undegraded/2022/3</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="23" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C20" s="32" t="n">
         <v>44881.5</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E20" s="26" t="n">
         <v>2022</v>
@@ -4826,10 +4785,10 @@
         <v>2</v>
       </c>
       <c r="I20" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J20" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K20" s="27" t="s">
         <v>55</v>
@@ -4855,22 +4814,23 @@
       <c r="R20" s="27" t="n">
         <v>47</v>
       </c>
-      <c r="S20" s="27" t="s">
-        <v>86</v>
+      <c r="S20" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D20,"/",E20,"/",F20)</f>
+        <v>tourist/2022/1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="23" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C21" s="32" t="n">
         <v>44881.5069444444</v>
       </c>
       <c r="D21" s="26" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E21" s="26" t="n">
         <v>2022</v>
@@ -4885,10 +4845,10 @@
         <v>2</v>
       </c>
       <c r="I21" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J21" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K21" s="27" t="s">
         <v>55</v>
@@ -4914,22 +4874,23 @@
       <c r="R21" s="27" t="n">
         <v>47</v>
       </c>
-      <c r="S21" s="27" t="s">
-        <v>86</v>
+      <c r="S21" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D21,"/",E21,"/",F21)</f>
+        <v>tourist/2022/1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="23" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C22" s="32" t="n">
         <v>44881.5138888889</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E22" s="26" t="n">
         <v>2022</v>
@@ -4944,10 +4905,10 @@
         <v>2</v>
       </c>
       <c r="I22" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J22" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K22" s="27" t="s">
         <v>55</v>
@@ -4973,22 +4934,23 @@
       <c r="R22" s="27" t="n">
         <v>47</v>
       </c>
-      <c r="S22" s="27" t="s">
-        <v>86</v>
+      <c r="S22" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D22,"/",E22,"/",F22)</f>
+        <v>tourist/2022/1</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="23" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C23" s="32" t="n">
         <v>44887.5034722222</v>
       </c>
       <c r="D23" s="26" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E23" s="26" t="n">
         <v>2022</v>
@@ -5003,10 +4965,10 @@
         <v>2</v>
       </c>
       <c r="I23" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J23" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K23" s="27" t="s">
         <v>55</v>
@@ -5032,22 +4994,23 @@
       <c r="R23" s="27" t="n">
         <v>47</v>
       </c>
-      <c r="S23" s="27" t="s">
-        <v>90</v>
+      <c r="S23" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D23,"/",E23,"/",F23)</f>
+        <v>tourist/2022/2</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="23" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C24" s="32" t="n">
         <v>44887.5104166667</v>
       </c>
       <c r="D24" s="26" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E24" s="26" t="n">
         <v>2022</v>
@@ -5062,10 +5025,10 @@
         <v>2</v>
       </c>
       <c r="I24" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J24" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K24" s="27" t="s">
         <v>55</v>
@@ -5091,22 +5054,23 @@
       <c r="R24" s="27" t="n">
         <v>47</v>
       </c>
-      <c r="S24" s="27" t="s">
-        <v>90</v>
+      <c r="S24" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D24,"/",E24,"/",F24)</f>
+        <v>tourist/2022/2</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="23" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C25" s="32" t="n">
         <v>44887.5173611111</v>
       </c>
       <c r="D25" s="26" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E25" s="26" t="n">
         <v>2022</v>
@@ -5121,10 +5085,10 @@
         <v>2</v>
       </c>
       <c r="I25" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J25" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K25" s="27" t="s">
         <v>55</v>
@@ -5150,22 +5114,23 @@
       <c r="R25" s="27" t="n">
         <v>47</v>
       </c>
-      <c r="S25" s="27" t="s">
-        <v>90</v>
+      <c r="S25" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D25,"/",E25,"/",F25)</f>
+        <v>tourist/2022/2</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="23" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B26" s="24" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C26" s="32" t="n">
         <v>44907.5034722222</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E26" s="26" t="n">
         <v>2022</v>
@@ -5180,10 +5145,10 @@
         <v>2</v>
       </c>
       <c r="I26" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J26" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K26" s="27" t="s">
         <v>55</v>
@@ -5209,22 +5174,23 @@
       <c r="R26" s="27" t="n">
         <v>47</v>
       </c>
-      <c r="S26" s="27" t="s">
-        <v>94</v>
+      <c r="S26" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D26,"/",E26,"/",F26)</f>
+        <v>tourist/2022/3</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="23" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="B27" s="24" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C27" s="32" t="n">
         <v>44907.5104166667</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E27" s="26" t="n">
         <v>2022</v>
@@ -5239,10 +5205,10 @@
         <v>2</v>
       </c>
       <c r="I27" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J27" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K27" s="27" t="s">
         <v>55</v>
@@ -5268,22 +5234,23 @@
       <c r="R27" s="27" t="n">
         <v>47</v>
       </c>
-      <c r="S27" s="27" t="s">
-        <v>94</v>
+      <c r="S27" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D27,"/",E27,"/",F27)</f>
+        <v>tourist/2022/3</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="23" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="B28" s="24" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C28" s="32" t="n">
         <v>44907.5173611111</v>
       </c>
       <c r="D28" s="26" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E28" s="26" t="n">
         <v>2022</v>
@@ -5298,10 +5265,10 @@
         <v>2</v>
       </c>
       <c r="I28" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J28" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K28" s="27" t="s">
         <v>55</v>
@@ -5327,22 +5294,23 @@
       <c r="R28" s="27" t="n">
         <v>47</v>
       </c>
-      <c r="S28" s="27" t="s">
-        <v>94</v>
+      <c r="S28" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D28,"/",E28,"/",F28)</f>
+        <v>tourist/2022/3</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="23" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="B29" s="24" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C29" s="32" t="n">
         <v>44243.5013888889</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E29" s="26" t="n">
         <v>2021</v>
@@ -5357,10 +5325,10 @@
         <v>2</v>
       </c>
       <c r="I29" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J29" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K29" s="27" t="s">
         <v>55</v>
@@ -5386,22 +5354,23 @@
       <c r="R29" s="27" t="n">
         <v>60</v>
       </c>
-      <c r="S29" s="27" t="s">
-        <v>98</v>
+      <c r="S29" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D29,"/",E29,"/",F29)</f>
+        <v>undegraded/2021/1</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="23" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="B30" s="24" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C30" s="32" t="n">
         <v>44243.5090277778</v>
       </c>
       <c r="D30" s="26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E30" s="26" t="n">
         <v>2021</v>
@@ -5416,10 +5385,10 @@
         <v>2</v>
       </c>
       <c r="I30" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J30" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K30" s="27" t="s">
         <v>55</v>
@@ -5445,22 +5414,23 @@
       <c r="R30" s="27" t="n">
         <v>60</v>
       </c>
-      <c r="S30" s="27" t="s">
-        <v>98</v>
+      <c r="S30" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D30,"/",E30,"/",F30)</f>
+        <v>undegraded/2021/1</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="23" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C31" s="32" t="n">
         <v>44243.5166666667</v>
       </c>
       <c r="D31" s="26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E31" s="26" t="n">
         <v>2021</v>
@@ -5475,10 +5445,10 @@
         <v>2</v>
       </c>
       <c r="I31" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J31" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K31" s="27" t="s">
         <v>55</v>
@@ -5504,22 +5474,23 @@
       <c r="R31" s="27" t="n">
         <v>60</v>
       </c>
-      <c r="S31" s="27" t="s">
-        <v>98</v>
+      <c r="S31" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D31,"/",E31,"/",F31)</f>
+        <v>undegraded/2021/1</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="23" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="C32" s="32" t="n">
         <v>44273.5034722222</v>
       </c>
       <c r="D32" s="26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E32" s="26" t="n">
         <v>2021</v>
@@ -5534,10 +5505,10 @@
         <v>2</v>
       </c>
       <c r="I32" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J32" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K32" s="27" t="s">
         <v>55</v>
@@ -5563,22 +5534,23 @@
       <c r="R32" s="27" t="n">
         <v>72</v>
       </c>
-      <c r="S32" s="27" t="s">
-        <v>102</v>
+      <c r="S32" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D32,"/",E32,"/",F32)</f>
+        <v>undegraded/2021/2</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="23" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="B33" s="24" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="C33" s="32" t="n">
         <v>44273.5111111111</v>
       </c>
       <c r="D33" s="26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E33" s="26" t="n">
         <v>2021</v>
@@ -5593,10 +5565,10 @@
         <v>2</v>
       </c>
       <c r="I33" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J33" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K33" s="27" t="s">
         <v>55</v>
@@ -5622,22 +5594,23 @@
       <c r="R33" s="27" t="n">
         <v>72</v>
       </c>
-      <c r="S33" s="27" t="s">
-        <v>102</v>
+      <c r="S33" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D33,"/",E33,"/",F33)</f>
+        <v>undegraded/2021/2</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="23" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="B34" s="24" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="C34" s="32" t="n">
         <v>44273.51875</v>
       </c>
       <c r="D34" s="26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E34" s="26" t="n">
         <v>2021</v>
@@ -5652,10 +5625,10 @@
         <v>2</v>
       </c>
       <c r="I34" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J34" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K34" s="27" t="s">
         <v>55</v>
@@ -5681,22 +5654,23 @@
       <c r="R34" s="27" t="n">
         <v>72</v>
       </c>
-      <c r="S34" s="27" t="s">
-        <v>102</v>
+      <c r="S34" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D34,"/",E34,"/",F34)</f>
+        <v>undegraded/2021/2</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="23" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="B35" s="24" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="C35" s="32" t="n">
         <v>44300.5034722222</v>
       </c>
       <c r="D35" s="26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E35" s="26" t="n">
         <v>2021</v>
@@ -5711,10 +5685,10 @@
         <v>2</v>
       </c>
       <c r="I35" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J35" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K35" s="27" t="s">
         <v>55</v>
@@ -5740,22 +5714,23 @@
       <c r="R35" s="27" t="n">
         <v>146</v>
       </c>
-      <c r="S35" s="27" t="s">
-        <v>106</v>
+      <c r="S35" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D35,"/",E35,"/",F35)</f>
+        <v>undegraded/2021/3</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="23" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="B36" s="24" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="C36" s="32" t="n">
         <v>44300.5111111111</v>
       </c>
       <c r="D36" s="26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E36" s="26" t="n">
         <v>2021</v>
@@ -5770,10 +5745,10 @@
         <v>2</v>
       </c>
       <c r="I36" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J36" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K36" s="27" t="s">
         <v>55</v>
@@ -5799,22 +5774,23 @@
       <c r="R36" s="27" t="n">
         <v>146</v>
       </c>
-      <c r="S36" s="27" t="s">
-        <v>106</v>
+      <c r="S36" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D36,"/",E36,"/",F36)</f>
+        <v>undegraded/2021/3</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="23" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="B37" s="24" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="C37" s="32" t="n">
         <v>44300.51875</v>
       </c>
       <c r="D37" s="26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E37" s="26" t="n">
         <v>2021</v>
@@ -5829,10 +5805,10 @@
         <v>2</v>
       </c>
       <c r="I37" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J37" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K37" s="27" t="s">
         <v>55</v>
@@ -5858,16 +5834,17 @@
       <c r="R37" s="27" t="n">
         <v>146</v>
       </c>
-      <c r="S37" s="27" t="s">
-        <v>106</v>
+      <c r="S37" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D37,"/",E37,"/",F37)</f>
+        <v>undegraded/2021/3</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="23" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="B38" s="24" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="C38" s="32" t="n">
         <v>44245.5041666667</v>
@@ -5917,16 +5894,17 @@
       <c r="R38" s="27" t="n">
         <v>46</v>
       </c>
-      <c r="S38" s="27" t="s">
-        <v>110</v>
+      <c r="S38" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D38,"/",E38,"/",F38)</f>
+        <v>boat/2021/1</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="23" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="B39" s="24" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="C39" s="32" t="n">
         <v>44245.5118055556</v>
@@ -5976,16 +5954,17 @@
       <c r="R39" s="27" t="n">
         <v>46</v>
       </c>
-      <c r="S39" s="27" t="s">
-        <v>110</v>
+      <c r="S39" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D39,"/",E39,"/",F39)</f>
+        <v>boat/2021/1</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="23" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="B40" s="24" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="C40" s="32" t="n">
         <v>44245.5194444444</v>
@@ -6035,16 +6014,17 @@
       <c r="R40" s="27" t="n">
         <v>46</v>
       </c>
-      <c r="S40" s="27" t="s">
-        <v>110</v>
+      <c r="S40" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D40,"/",E40,"/",F40)</f>
+        <v>boat/2021/1</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="23" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="B41" s="24" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="C41" s="32" t="n">
         <v>44271.5027777778</v>
@@ -6074,7 +6054,7 @@
         <v>55</v>
       </c>
       <c r="L41" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M41" s="27" t="s">
         <v>56</v>
@@ -6094,16 +6074,17 @@
       <c r="R41" s="27" t="n">
         <v>42</v>
       </c>
-      <c r="S41" s="27" t="s">
-        <v>114</v>
+      <c r="S41" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D41,"/",E41,"/",F41)</f>
+        <v>boat/2021/2</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="23" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="B42" s="24" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="C42" s="32" t="n">
         <v>44271.5104166667</v>
@@ -6153,16 +6134,17 @@
       <c r="R42" s="27" t="n">
         <v>42</v>
       </c>
-      <c r="S42" s="27" t="s">
-        <v>114</v>
+      <c r="S42" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D42,"/",E42,"/",F42)</f>
+        <v>boat/2021/2</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="23" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="B43" s="24" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="C43" s="32" t="n">
         <v>44271.5180555556</v>
@@ -6212,16 +6194,17 @@
       <c r="R43" s="27" t="n">
         <v>42</v>
       </c>
-      <c r="S43" s="27" t="s">
-        <v>114</v>
+      <c r="S43" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D43,"/",E43,"/",F43)</f>
+        <v>boat/2021/2</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="23" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="B44" s="24" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="C44" s="32" t="n">
         <v>44305.5027777778</v>
@@ -6271,16 +6254,17 @@
       <c r="R44" s="27" t="n">
         <v>90</v>
       </c>
-      <c r="S44" s="27" t="s">
-        <v>118</v>
+      <c r="S44" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D44,"/",E44,"/",F44)</f>
+        <v>boat/2021/3</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="23" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="B45" s="24" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="C45" s="32" t="n">
         <v>44305.5104166667</v>
@@ -6310,7 +6294,7 @@
         <v>55</v>
       </c>
       <c r="L45" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M45" s="27" t="s">
         <v>56</v>
@@ -6330,16 +6314,17 @@
       <c r="R45" s="27" t="n">
         <v>90</v>
       </c>
-      <c r="S45" s="27" t="s">
-        <v>118</v>
+      <c r="S45" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D45,"/",E45,"/",F45)</f>
+        <v>boat/2021/3</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="23" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="B46" s="24" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="C46" s="32" t="n">
         <v>44305.5180555556</v>
@@ -6389,22 +6374,23 @@
       <c r="R46" s="27" t="n">
         <v>90</v>
       </c>
-      <c r="S46" s="27" t="s">
-        <v>118</v>
+      <c r="S46" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D46,"/",E46,"/",F46)</f>
+        <v>boat/2021/3</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="23" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="B47" s="24" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="C47" s="32" t="n">
         <v>44243.5055555556</v>
       </c>
       <c r="D47" s="26" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E47" s="26" t="n">
         <v>2021</v>
@@ -6419,10 +6405,10 @@
         <v>2</v>
       </c>
       <c r="I47" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J47" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K47" s="27" t="s">
         <v>55</v>
@@ -6448,22 +6434,23 @@
       <c r="R47" s="27" t="n">
         <v>54</v>
       </c>
-      <c r="S47" s="27" t="s">
-        <v>122</v>
+      <c r="S47" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D47,"/",E47,"/",F47)</f>
+        <v>tourist/2021/1</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="23" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="B48" s="24" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="C48" s="32" t="n">
         <v>44243.5131944445</v>
       </c>
       <c r="D48" s="26" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E48" s="26" t="n">
         <v>2021</v>
@@ -6478,10 +6465,10 @@
         <v>2</v>
       </c>
       <c r="I48" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J48" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K48" s="27" t="s">
         <v>55</v>
@@ -6507,22 +6494,23 @@
       <c r="R48" s="27" t="n">
         <v>54</v>
       </c>
-      <c r="S48" s="27" t="s">
-        <v>122</v>
+      <c r="S48" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D48,"/",E48,"/",F48)</f>
+        <v>tourist/2021/1</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="23" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B49" s="24" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="C49" s="32" t="n">
         <v>44243.5208333333</v>
       </c>
       <c r="D49" s="26" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E49" s="26" t="n">
         <v>2021</v>
@@ -6537,10 +6525,10 @@
         <v>2</v>
       </c>
       <c r="I49" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J49" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K49" s="27" t="s">
         <v>55</v>
@@ -6566,22 +6554,23 @@
       <c r="R49" s="27" t="n">
         <v>54</v>
       </c>
-      <c r="S49" s="27" t="s">
-        <v>122</v>
+      <c r="S49" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D49,"/",E49,"/",F49)</f>
+        <v>tourist/2021/1</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="23" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="B50" s="24" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="C50" s="32" t="n">
         <v>44273.5</v>
       </c>
       <c r="D50" s="26" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E50" s="26" t="n">
         <v>2021</v>
@@ -6596,10 +6585,10 @@
         <v>2</v>
       </c>
       <c r="I50" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J50" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K50" s="27" t="s">
         <v>55</v>
@@ -6625,22 +6614,23 @@
       <c r="R50" s="27" t="n">
         <v>63</v>
       </c>
-      <c r="S50" s="27" t="s">
-        <v>126</v>
+      <c r="S50" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D50,"/",E50,"/",F50)</f>
+        <v>tourist/2021/2</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="23" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="B51" s="24" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="C51" s="32" t="n">
         <v>44273.5076388889</v>
       </c>
       <c r="D51" s="26" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E51" s="26" t="n">
         <v>2021</v>
@@ -6655,10 +6645,10 @@
         <v>2</v>
       </c>
       <c r="I51" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J51" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K51" s="27" t="s">
         <v>55</v>
@@ -6684,22 +6674,23 @@
       <c r="R51" s="27" t="n">
         <v>63</v>
       </c>
-      <c r="S51" s="27" t="s">
-        <v>126</v>
+      <c r="S51" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D51,"/",E51,"/",F51)</f>
+        <v>tourist/2021/2</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="23" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="B52" s="24" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="C52" s="32" t="n">
         <v>44273.5152777778</v>
       </c>
       <c r="D52" s="26" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E52" s="26" t="n">
         <v>2021</v>
@@ -6714,10 +6705,10 @@
         <v>2</v>
       </c>
       <c r="I52" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J52" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K52" s="27" t="s">
         <v>55</v>
@@ -6743,22 +6734,23 @@
       <c r="R52" s="27" t="n">
         <v>63</v>
       </c>
-      <c r="S52" s="27" t="s">
-        <v>126</v>
+      <c r="S52" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D52,"/",E52,"/",F52)</f>
+        <v>tourist/2021/2</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="23" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="B53" s="24" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="C53" s="32" t="n">
         <v>44299.5069444445</v>
       </c>
       <c r="D53" s="26" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E53" s="26" t="n">
         <v>2021</v>
@@ -6773,10 +6765,10 @@
         <v>2</v>
       </c>
       <c r="I53" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J53" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K53" s="27" t="s">
         <v>55</v>
@@ -6802,22 +6794,23 @@
       <c r="R53" s="27" t="n">
         <v>86</v>
       </c>
-      <c r="S53" s="27" t="s">
-        <v>130</v>
+      <c r="S53" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D53,"/",E53,"/",F53)</f>
+        <v>tourist/2021/3</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="23" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="B54" s="24" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="C54" s="32" t="n">
         <v>44299.5145833333</v>
       </c>
       <c r="D54" s="26" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E54" s="26" t="n">
         <v>2021</v>
@@ -6832,10 +6825,10 @@
         <v>2</v>
       </c>
       <c r="I54" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J54" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K54" s="27" t="s">
         <v>55</v>
@@ -6861,22 +6854,23 @@
       <c r="R54" s="27" t="n">
         <v>86</v>
       </c>
-      <c r="S54" s="27" t="s">
-        <v>130</v>
+      <c r="S54" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D54,"/",E54,"/",F54)</f>
+        <v>tourist/2021/3</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="23" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="B55" s="24" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="C55" s="32" t="n">
         <v>44299.5222222222</v>
       </c>
       <c r="D55" s="26" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E55" s="26" t="n">
         <v>2021</v>
@@ -6891,10 +6885,10 @@
         <v>2</v>
       </c>
       <c r="I55" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J55" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K55" s="27" t="s">
         <v>55</v>
@@ -6920,8 +6914,9 @@
       <c r="R55" s="27" t="n">
         <v>86</v>
       </c>
-      <c r="S55" s="27" t="s">
-        <v>130</v>
+      <c r="S55" s="27" t="str">
+        <f aca="false">_xlfn.CONCAT(D55,"/",E55,"/",F55)</f>
+        <v>tourist/2021/3</v>
       </c>
     </row>
   </sheetData>
@@ -6959,18 +6954,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="28" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="33" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="B2" s="34" t="n">
         <v>70</v>
@@ -7026,15 +7021,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="28" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="33" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="B2" s="34" t="n">
         <v>15</v>
@@ -7085,18 +7080,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="28" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="33" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="B2" s="31" t="n">
         <v>44562.5</v>
@@ -7107,7 +7102,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="33" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
       <c r="B3" s="31" t="n">
         <v>44881.5</v>
@@ -7118,7 +7113,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="33" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="B4" s="32" t="n">
         <v>44887.5</v>
@@ -7129,7 +7124,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="33" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
       <c r="B5" s="32" t="n">
         <v>44907.5</v>
@@ -7174,27 +7169,27 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="28" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="F1" s="28" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="33" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="B2" s="31" t="n">
         <v>44881.5</v>
@@ -7203,18 +7198,18 @@
         <v>44882.5034722222</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F2" s="31" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="33" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="B3" s="31" t="n">
         <v>44887.5</v>
@@ -7223,18 +7218,18 @@
         <v>44888.5034722222</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="E3" s="31" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F3" s="31" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="35" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="B4" s="31" t="n">
         <v>44907.5</v>
@@ -7243,13 +7238,13 @@
         <v>44908.5034722222</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F4" s="31" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7308,21 +7303,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="40" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="B1" s="40" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="C1" s="40" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="D1" s="40" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="36" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
       <c r="B2" s="37" t="n">
         <v>0</v>
@@ -7331,7 +7326,7 @@
         <v>1000</v>
       </c>
       <c r="D2" s="38" t="s">
-        <v>160</v>
+        <v>56</v>
       </c>
       <c r="E2" s="39" t="str">
         <f aca="false">VLOOKUP(A2,ListExtractors!$A$2:$B$1048576,2,0)</f>
@@ -7378,12 +7373,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="40" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="41" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="B2" s="39" t="str">
         <f aca="false">VLOOKUP(A2,ListDigesters!$A$2:$B$1048576,2,0)</f>
@@ -7392,7 +7387,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="41" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
       <c r="B3" s="39" t="str">
         <f aca="false">VLOOKUP(A3,ListDigesters!$A$2:$B$1048576,2,0)</f>

</xml_diff>

<commit_message>
fix(Examples): Update campaigns configurations and datasets
</commit_message>
<xml_diff>
--- a/examples/campaigns/coral-reef-light/coral-reef-light.xlsx
+++ b/examples/campaigns/coral-reef-light/coral-reef-light.xlsx
@@ -37,7 +37,7 @@
 <file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>BS</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0">
@@ -182,7 +182,7 @@
 <file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>BS</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0">
@@ -258,7 +258,7 @@
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>BS</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0">
@@ -308,7 +308,7 @@
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>BS</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0">
@@ -357,7 +357,7 @@
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>BS</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0">
@@ -393,7 +393,7 @@
 <file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>BS</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0">
@@ -442,7 +442,7 @@
 <file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>BS</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0">
@@ -530,7 +530,7 @@
 <file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>BS</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0">
@@ -593,7 +593,7 @@
 <file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>BS</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0">
@@ -618,7 +618,7 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="194">
   <si>
     <t xml:space="preserve">SoundScapeExplorer
-Version 12</t>
+Version 13</t>
   </si>
   <si>
     <t xml:space="preserve">Instructions</t>

</xml_diff>